<commit_message>
WhatsApp: confirmaciones + recordatorios
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\salon_agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89AB896-E8CA-4BA3-B9D4-6B6590F615FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BC675-4631-4C89-B216-578F16A89993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
   </bookViews>
@@ -489,57 +489,57 @@
   <dimension ref="R7:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Z11" sqref="Z11"/>
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="7" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R11" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="18:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
       <c r="R24" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Actualiza landing, servicios y testimonios
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\salon_agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991BC675-4631-4C89-B216-578F16A89993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A1339-4059-4045-8426-9645E0090527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>http://127.0.0.1:8000/reservar/</t>
   </si>
@@ -66,19 +66,187 @@
   </si>
   <si>
     <t>pip install django</t>
+  </si>
+  <si>
+    <t>cd "C:\Users\jvz16\salon_agenda"</t>
+  </si>
+  <si>
+    <t># si tu carpeta es .venv</t>
+  </si>
+  <si>
+    <t>.\.venv\Scripts\Activate.ps1</t>
+  </si>
+  <si>
+    <t># si tu carpeta es venv</t>
+  </si>
+  <si>
+    <t>.\venv\Scripts\Activate.ps1</t>
+  </si>
+  <si>
+    <t>py -m venv .venv</t>
+  </si>
+  <si>
+    <t>python -m pip install --upgrade pip</t>
+  </si>
+  <si>
+    <t>pip install -r requirements.txt</t>
+  </si>
+  <si>
+    <t># si no tienes requirements.txt, instala directo:</t>
+  </si>
+  <si>
+    <t># pip install "Django&gt;=4.2,&lt;5"</t>
+  </si>
+  <si>
+    <t>pip install Pillow</t>
+  </si>
+  <si>
+    <t>Producción (Render)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Landing / Reservar: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>https://salon-nadira.onrender.com/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Servicios: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>https://salon-nadira.onrender.com/servicios/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testimonios: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>https://salon-nadira.onrender.com/testimonios/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Admin: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>https://salon-nadira.onrender.com/admin/</t>
+    </r>
+  </si>
+  <si>
+    <t>Local (tu PC)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Landing / Reservar: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>http://127.0.0.1:8000/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Servicios: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>http://127.0.0.1:8000/servicios/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Testimonios: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>http://127.0.0.1:8000/testimonios/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Admin: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>http://127.0.0.1:8000/admin/</t>
+    </r>
+  </si>
+  <si>
+    <t>jvz</t>
+  </si>
+  <si>
+    <t>jvz123</t>
+  </si>
+  <si>
+    <t>Clave</t>
+  </si>
+  <si>
+    <t>Usuario</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -101,8 +269,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -132,8 +306,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>515419</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>172198</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>148385</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -486,62 +660,211 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD43CF-C200-474D-8D07-6F8BDE2B25EE}">
-  <dimension ref="R7:R24"/>
+  <dimension ref="R7:Y52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W24" sqref="W24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X52" sqref="X52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="7" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="18:24">
       <c r="R7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="18:24">
       <c r="R8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="18:24">
       <c r="R9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="18:24">
       <c r="R10" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="18:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="18:24">
       <c r="R11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="18:24">
       <c r="R12" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="18:24">
+      <c r="X14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="18:24">
+      <c r="X15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="18:24">
+      <c r="X17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="18:24">
       <c r="R18" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="18:24">
+      <c r="X19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="18:24">
       <c r="R20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="18:24">
       <c r="R22" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="18:18" x14ac:dyDescent="0.25">
+      <c r="X22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="18:24">
       <c r="R24" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="18:24">
+      <c r="X25" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="18:24">
+      <c r="X26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="18:24" ht="31.5">
+      <c r="X28" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="18:24">
+      <c r="X29" s="2"/>
+    </row>
+    <row r="30" spans="18:24">
+      <c r="X30" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="18:24">
+      <c r="X31" s="2"/>
+    </row>
+    <row r="32" spans="18:24">
+      <c r="X32" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="24:24">
+      <c r="X33" s="2"/>
+    </row>
+    <row r="34" spans="24:24">
+      <c r="X34" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="24:24">
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="24:24">
+      <c r="X36" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="24:24" ht="31.5">
+      <c r="X38" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="24:24">
+      <c r="X39" s="2"/>
+    </row>
+    <row r="40" spans="24:24">
+      <c r="X40" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="24:24">
+      <c r="X41" s="2"/>
+    </row>
+    <row r="42" spans="24:24">
+      <c r="X42" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="43" spans="24:24">
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="24:24">
+      <c r="X44" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="24:24">
+      <c r="X45" s="2"/>
+    </row>
+    <row r="46" spans="24:24">
+      <c r="X46" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="24:25">
+      <c r="X49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="24:25">
+      <c r="X51" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="24:25">
+      <c r="X52" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modelos Testimonial/BeforeAfter y migraciones
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\salon_agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279A1339-4059-4045-8426-9645E0090527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D3EA29-9137-4BAD-8C17-6247E24D992E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
   <si>
     <t>http://127.0.0.1:8000/reservar/</t>
   </si>
@@ -221,6 +221,30 @@
   </si>
   <si>
     <t>Usuario</t>
+  </si>
+  <si>
+    <t>python manage.py changepassword jvz16</t>
+  </si>
+  <si>
+    <t>python manage.py shell</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt; from django.contrib.auth.models import User</t>
+  </si>
+  <si>
+    <t>&gt;&gt;&gt; User.objects.all()</t>
+  </si>
+  <si>
+    <t>git status</t>
+  </si>
+  <si>
+    <t>git add -A</t>
+  </si>
+  <si>
+    <t>git commit -m "Actualiza landing, servicios y testimonios"</t>
+  </si>
+  <si>
+    <t>git push origin main   # o la rama que usa Render</t>
   </si>
 </sst>
 </file>
@@ -660,10 +684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD43CF-C200-474D-8D07-6F8BDE2B25EE}">
-  <dimension ref="R7:Y52"/>
+  <dimension ref="R7:Y63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="X52" sqref="X52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="X44" sqref="X44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -867,6 +891,51 @@
         <v>32</v>
       </c>
     </row>
+    <row r="53" spans="24:25">
+      <c r="X53" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="54" spans="24:25">
+      <c r="X54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="55" spans="24:25">
+      <c r="X55" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="24:25">
+      <c r="X56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="24:25">
+      <c r="X58" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="24:25">
+      <c r="X59" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="24:25">
+      <c r="X60" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="61" spans="24:25">
+      <c r="X61" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="63" spans="24:25">
+      <c r="X63" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Update Nadira Fashion: HomeBackground, styles and views
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\salon_agenda\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\Proyectos\salon_agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C075AF8-425E-4E7B-9A36-682BBF17942C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D0D00D7-DE65-42F5-9249-81BBF120540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>http://127.0.0.1:8000/reservar/</t>
   </si>
@@ -62,25 +62,13 @@
     <t>pip install twilio</t>
   </si>
   <si>
-    <t>cd C:\Users\jvz16\salon_agenda\</t>
-  </si>
-  <si>
     <t>pip install django</t>
   </si>
   <si>
-    <t>cd "C:\Users\jvz16\salon_agenda"</t>
-  </si>
-  <si>
     <t># si tu carpeta es .venv</t>
   </si>
   <si>
     <t>.\.venv\Scripts\Activate.ps1</t>
-  </si>
-  <si>
-    <t># si tu carpeta es venv</t>
-  </si>
-  <si>
-    <t>.\venv\Scripts\Activate.ps1</t>
   </si>
   <si>
     <t>py -m venv .venv</t>
@@ -248,6 +236,105 @@
   </si>
   <si>
     <t>https://TU-SERVICIO.onrender.com/</t>
+  </si>
+  <si>
+    <t>Cómo arrancar:</t>
+  </si>
+  <si>
+    <t>1. python -m venv .venv</t>
+  </si>
+  <si>
+    <t>2. source .venv/bin/activate   (Windows: .venv\Scripts\activate)</t>
+  </si>
+  <si>
+    <t>3. pip install -r requirements.txt</t>
+  </si>
+  <si>
+    <t>4. python manage.py migrate</t>
+  </si>
+  <si>
+    <t>5. python manage.py createsuperuser   (crear admin)</t>
+  </si>
+  <si>
+    <t>6. python manage.py runserver</t>
+  </si>
+  <si>
+    <t>cd "C:\Users\jvz16\ordero"</t>
+  </si>
+  <si>
+    <t>python -m venv .venv</t>
+  </si>
+  <si>
+    <t>.venv\Scripts\activate</t>
+  </si>
+  <si>
+    <t>http://127.0.0.1:8000/</t>
+  </si>
+  <si>
+    <t>Setup: http://127.0.0.1:8000/setup/</t>
+  </si>
+  <si>
+    <t>Salón: http://127.0.0.1:8000/orders/floor/</t>
+  </si>
+  <si>
+    <t>Menú: http://127.0.0.1:8000/menu/editor/</t>
+  </si>
+  <si>
+    <t>Cocina: http://127.0.0.1:8000/kitchen/board/</t>
+  </si>
+  <si>
+    <t>Resumen: http://127.0.0.1:8000/reports/daily/</t>
+  </si>
+  <si>
+    <t>Admin: http://127.0.0.1:8000/admin/</t>
+  </si>
+  <si>
+    <t>Issue con sillas</t>
+  </si>
+  <si>
+    <t>No se muestra resumen despues de haber cerrado mesas</t>
+  </si>
+  <si>
+    <t>Disposicion geografica de mesas/sillas</t>
+  </si>
+  <si>
+    <t>Diferentes permisos en la app (dueño vs salonero vs cocina) - solo dueño edita menu</t>
+  </si>
+  <si>
+    <t>Asociar nombre de persona a ticket</t>
+  </si>
+  <si>
+    <t>Estado (emoji) de la mesa al lado de la mesa</t>
+  </si>
+  <si>
+    <t>Panel desarrollador: yo - administro restaurantes asociados</t>
+  </si>
+  <si>
+    <t>Panel editor: dueño rest - edita menu, agrega saloneros, ve resultados</t>
+  </si>
+  <si>
+    <t>Panel usuario: salones y cocina</t>
+  </si>
+  <si>
+    <t>cd "C:\Users\jvz16\Proyectos\salon_agenda"</t>
+  </si>
+  <si>
+    <t>&amp; "C:\Users\jvz16\anaconda3\python.exe" -m venv .venv</t>
+  </si>
+  <si>
+    <t>cd C:\Users\jvz16\Proyectos\salon_agenda</t>
+  </si>
+  <si>
+    <t>Remove-Item Env:DATABASE_URL -ErrorAction SilentlyContinue</t>
+  </si>
+  <si>
+    <t>$env:DATABASE_URL</t>
+  </si>
+  <si>
+    <t>python -m pip install -r requirements.txt</t>
+  </si>
+  <si>
+    <t>python -m pip install Pillow</t>
   </si>
 </sst>
 </file>
@@ -687,192 +774,289 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD43CF-C200-474D-8D07-6F8BDE2B25EE}">
-  <dimension ref="R7:Y63"/>
+  <dimension ref="R2:AE77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R64" sqref="R64"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
-    <row r="7" spans="18:24">
-      <c r="R7" t="s">
-        <v>8</v>
-      </c>
+    <row r="2" spans="18:31">
+      <c r="X2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="18:31">
+      <c r="X3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="18:31">
+      <c r="X4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="18:31">
+      <c r="X5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="18:31">
+      <c r="X6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="18:31">
       <c r="X7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="18:24">
+        <v>72</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="18:31">
       <c r="R8" t="s">
         <v>1</v>
       </c>
       <c r="X8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="18:24">
+        <v>66</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="18:31">
       <c r="R9" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" t="s">
         <v>9</v>
       </c>
-      <c r="X9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="18:24">
+      <c r="AE9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="18:31">
       <c r="R10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="18:24">
+      <c r="X10" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="18:31">
       <c r="R11" t="s">
         <v>3</v>
       </c>
       <c r="X11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="18:24">
+        <v>67</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="18:31">
       <c r="R12" t="s">
         <v>7</v>
       </c>
-      <c r="X12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="18:24">
+      <c r="AE12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="18:31">
+      <c r="AE13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="18:31">
       <c r="X14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="18:24">
-      <c r="X15" t="s">
+        <v>11</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="18:31">
+      <c r="AE15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="18:31">
+      <c r="AE16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="18:31">
+      <c r="X17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="18:24">
-      <c r="X17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="18:24">
+    <row r="18" spans="18:31">
       <c r="R18" t="s">
         <v>4</v>
       </c>
       <c r="X18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="18:24">
+        <v>13</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="18:31">
       <c r="X19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="18:24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="18:31">
       <c r="R20" t="s">
         <v>5</v>
       </c>
       <c r="X20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="18:24">
+        <v>15</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="18:31">
       <c r="R22" t="s">
         <v>6</v>
       </c>
       <c r="X22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="24" spans="18:24">
+        <v>16</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="18:31">
       <c r="R24" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="18:24">
+      <c r="AE24" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="25" spans="18:31">
       <c r="X25" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="18:24">
+    <row r="26" spans="18:31">
       <c r="X26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="18:24" ht="31.5">
+      <c r="AE26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="18:31" ht="31.2">
       <c r="X28" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="18:31">
+      <c r="X29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="18:31">
+      <c r="X30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="18:31">
+      <c r="X31" s="2"/>
+      <c r="AE31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="18:31">
+      <c r="X32" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="33" spans="24:31">
+      <c r="X33" s="2"/>
+      <c r="AE33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="24:31">
+      <c r="X34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="24:31">
+      <c r="X35" s="2"/>
+      <c r="AE35" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="24:31">
+      <c r="X36" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="18:24">
-      <c r="X29" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="18:24">
-      <c r="X30" s="2" t="s">
+    <row r="37" spans="24:31">
+      <c r="AE37" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="24:31" ht="31.2">
+      <c r="X38" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="18:24">
-      <c r="X31" s="2"/>
-    </row>
-    <row r="32" spans="18:24">
-      <c r="X32" s="2" t="s">
+      <c r="AE38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="24:31">
+      <c r="X39" s="2"/>
+      <c r="AE39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="24:31">
+      <c r="X40" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="24:24">
-      <c r="X33" s="2"/>
-    </row>
-    <row r="34" spans="24:24">
-      <c r="X34" s="2" t="s">
+    <row r="41" spans="24:31">
+      <c r="X41" s="2"/>
+    </row>
+    <row r="42" spans="24:31">
+      <c r="X42" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="24:24">
-      <c r="X35" s="2"/>
-    </row>
-    <row r="36" spans="24:24">
-      <c r="X36" s="2" t="s">
+    <row r="43" spans="24:31">
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="24:31">
+      <c r="X44" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="24:24" ht="31.5">
-      <c r="X38" s="1" t="s">
+    <row r="45" spans="24:31">
+      <c r="X45" s="2"/>
+    </row>
+    <row r="46" spans="24:31">
+      <c r="X46" s="2" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="24:24">
-      <c r="X39" s="2"/>
-    </row>
-    <row r="40" spans="24:24">
-      <c r="X40" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="41" spans="24:24">
-      <c r="X41" s="2"/>
-    </row>
-    <row r="42" spans="24:24">
-      <c r="X42" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="24:24">
-      <c r="X43" s="2"/>
-    </row>
-    <row r="44" spans="24:24">
-      <c r="X44" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="24:24">
-      <c r="X45" s="2"/>
-    </row>
-    <row r="46" spans="24:24">
-      <c r="X46" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="49" spans="24:25">
@@ -882,63 +1066,98 @@
     </row>
     <row r="51" spans="24:25">
       <c r="X51" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="Y51" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="24:25">
       <c r="X52" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="Y52" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="53" spans="24:25">
       <c r="X53" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="24:25">
       <c r="X54" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="24:25">
       <c r="X55" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="24:25">
       <c r="X56" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="58" spans="24:25">
       <c r="X58" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="59" spans="24:25">
       <c r="X59" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="60" spans="24:25">
       <c r="X60" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="61" spans="24:25">
       <c r="X61" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="63" spans="24:25">
       <c r="X63" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="71" spans="24:24">
+      <c r="X71" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="72" spans="24:24">
+      <c r="X72" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="73" spans="24:24">
+      <c r="X73" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="74" spans="24:24">
+      <c r="X74" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="75" spans="24:24">
+      <c r="X75" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="24:24">
+      <c r="X76" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="77" spans="24:24">
+      <c r="X77" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualiza formato para Clientes VIP
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvz16\Proyectos\salon_agenda\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009DB47D-CB88-4EE4-A5BE-623EC8754A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A919411C-2B20-4F7B-823A-0FAEB5CEBCCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7156CD1D-D3BB-44C2-9761-0A4246B0D336}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
   <si>
     <t>http://127.0.0.1:8000/reservar/</t>
   </si>
@@ -229,9 +229,6 @@
     <t>git add -A</t>
   </si>
   <si>
-    <t>git commit -m "Actualiza landing, servicios y testimonios"</t>
-  </si>
-  <si>
     <t>git push origin main   # o la rama que usa Render</t>
   </si>
   <si>
@@ -395,6 +392,12 @@
   </si>
   <si>
     <t>Cambiar "© Salón Nadira" por " Centro de Belleza &amp; Spa Nadira Fashion"</t>
+  </si>
+  <si>
+    <t>No PROMOS, si PAQUETES</t>
+  </si>
+  <si>
+    <t>git commit -m "Actualiza formato para Clientes VIP"</t>
   </si>
 </sst>
 </file>
@@ -850,119 +853,122 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36CD43CF-C200-474D-8D07-6F8BDE2B25EE}">
   <dimension ref="R2:AT77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+    <sheetView tabSelected="1" topLeftCell="O28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AE56" sqref="AE56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="2" spans="18:46">
       <c r="R2" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="X2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AT2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="18:46">
       <c r="R3" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X3" t="s">
         <v>10</v>
       </c>
       <c r="AL3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AT3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="18:46">
       <c r="R4" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="X4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AL4" t="s">
         <v>10</v>
       </c>
       <c r="AT4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="18:46">
       <c r="R5" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="X5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AL5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AT5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="18:46">
       <c r="R6" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="X6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AL6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AT6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="18:46">
       <c r="R7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="X7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AE7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AT7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="18:46">
       <c r="R8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AE8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="18:46">
       <c r="R9" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="X9" t="s">
         <v>9</v>
       </c>
       <c r="AE9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AL9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="10" spans="18:46">
+      <c r="R10" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="X10" t="s">
         <v>10</v>
       </c>
@@ -970,12 +976,12 @@
         <v>13</v>
       </c>
       <c r="AL10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="18:46">
       <c r="X11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE11" t="s">
         <v>2</v>
@@ -991,7 +997,7 @@
         <v>4</v>
       </c>
       <c r="AL13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="18:46">
@@ -999,10 +1005,10 @@
         <v>11</v>
       </c>
       <c r="AE14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AL14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="18:46">
@@ -1012,7 +1018,7 @@
     </row>
     <row r="16" spans="18:46">
       <c r="AE16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="18:31">
@@ -1025,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="AE18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="18:31">
@@ -1038,7 +1044,7 @@
         <v>15</v>
       </c>
       <c r="AE20" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="18:31">
@@ -1046,7 +1052,7 @@
         <v>16</v>
       </c>
       <c r="AE22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="18:31">
@@ -1059,7 +1065,7 @@
         <v>8</v>
       </c>
       <c r="AE24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="18:31">
@@ -1078,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="AE26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="18:31">
@@ -1093,7 +1099,7 @@
     </row>
     <row r="29" spans="18:31">
       <c r="X29" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="18:31">
@@ -1101,13 +1107,13 @@
         <v>18</v>
       </c>
       <c r="AE30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="18:31">
       <c r="X31" s="2"/>
       <c r="AE31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="18:31">
@@ -1115,7 +1121,7 @@
         <v>19</v>
       </c>
       <c r="AE32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="18:31">
@@ -1124,7 +1130,7 @@
       </c>
       <c r="X33" s="2"/>
       <c r="AE33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="18:31">
@@ -1132,7 +1138,7 @@
         <v>20</v>
       </c>
       <c r="AE34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="18:31">
@@ -1141,7 +1147,7 @@
       </c>
       <c r="X35" s="2"/>
       <c r="AE35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="18:31">
@@ -1154,7 +1160,7 @@
         <v>6</v>
       </c>
       <c r="AE37" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="18:31" ht="31.5">
@@ -1162,7 +1168,7 @@
         <v>22</v>
       </c>
       <c r="AE38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="18:31">
@@ -1171,7 +1177,7 @@
       </c>
       <c r="X39" s="2"/>
       <c r="AE39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="18:31">
@@ -1256,12 +1262,12 @@
     </row>
     <row r="60" spans="24:25">
       <c r="X60" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="24:25">
       <c r="X61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="24:25">
@@ -1271,37 +1277,37 @@
     </row>
     <row r="71" spans="24:24">
       <c r="X71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="72" spans="24:24">
       <c r="X72" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="73" spans="24:24">
       <c r="X73" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="74" spans="24:24">
       <c r="X74" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="75" spans="24:24">
       <c r="X75" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="76" spans="24:24">
       <c r="X76" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="24:24">
       <c r="X77" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>